<commit_message>
Change from Height To Normalized Units
</commit_message>
<xml_diff>
--- a/positions.xlsx
+++ b/positions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sag22id\Documents\Projects\GCA\gaze_avoidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63504EA-D643-40CA-9699-32A953119144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0A075E-8608-4269-A66A-F1D378F0A74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="1671" windowWidth="14383" windowHeight="9815" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -41,18 +41,6 @@
     <t>position</t>
   </si>
   <si>
-    <t>(-0.5, 0.2)</t>
-  </si>
-  <si>
-    <t>(0.5, 0.2)</t>
-  </si>
-  <si>
-    <t>(-0.5, -0.2)</t>
-  </si>
-  <si>
-    <t>(0.5, -0.2)</t>
-  </si>
-  <si>
     <t>trialtype</t>
   </si>
   <si>
@@ -66,6 +54,18 @@
   </si>
   <si>
     <t>cs_minus_ns</t>
+  </si>
+  <si>
+    <t>(-0.6, 0.6)</t>
+  </si>
+  <si>
+    <t>(-0.6, -0.6)</t>
+  </si>
+  <si>
+    <t>(0.6, 0.6)</t>
+  </si>
+  <si>
+    <t>(0.6, -0.6)</t>
   </si>
 </sst>
 </file>
@@ -420,148 +420,148 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hide mouse, fix ROIs (size and position)
</commit_message>
<xml_diff>
--- a/positions.xlsx
+++ b/positions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sag22id\Documents\Projects\GCA\gaze_avoidance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Projects\GCA\gaze_avoidance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0A075E-8608-4269-A66A-F1D378F0A74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{EE2D1E65-ECCA-4926-8829-64F5B2CF654A}"/>
+    <workbookView xWindow="-38505" yWindow="-105" windowWidth="38625" windowHeight="21225"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,22 +55,22 @@
     <t>cs_minus_ns</t>
   </si>
   <si>
-    <t>(-0.6, 0.6)</t>
-  </si>
-  <si>
-    <t>(-0.6, -0.6)</t>
-  </si>
-  <si>
-    <t>(0.6, 0.6)</t>
-  </si>
-  <si>
-    <t>(0.6, -0.6)</t>
+    <t>(-0.7, 0.5)</t>
+  </si>
+  <si>
+    <t>(-0.7, -0.5)</t>
+  </si>
+  <si>
+    <t>(0.7, 0.5)</t>
+  </si>
+  <si>
+    <t>(0.7, -0.5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,19 +415,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D442166-CB98-4944-BF44-DA0360414B46}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -444,7 +443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -452,7 +451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -460,7 +459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -468,7 +467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -476,7 +475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -484,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -492,7 +491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -500,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -508,7 +507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -516,7 +515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -524,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -532,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -540,7 +539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -548,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -556,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>

</xml_diff>